<commit_message>
work on TGS-560 removing some redundant images (en.) added links to sheets in connectors and parameters.xlsx
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -671,7 +671,7 @@
     <t xml:space="preserve">CONNECTORS</t>
   </si>
   <si>
-    <t xml:space="preserve">Network connector</t>
+    <t xml:space="preserve">Mains connector</t>
   </si>
   <si>
     <t xml:space="preserve">DC bus connector</t>
@@ -722,13 +722,13 @@
     <t xml:space="preserve">Recommended circuit breaker</t>
   </si>
   <si>
-    <t xml:space="preserve">AC IN connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 4pin WEIDMÜLLER BVF 7.62HP/04/180F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 6pin WEIDMÜLLER BVF 7.62HP/06/180F</t>
+    <t xml:space="preserve">Logic power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 4pin WEIDMÜLLER BVZ 7.62HP/04/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 6pin WEIDMÜLLER BVZ 7.62HP/06/180F</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 4pin WEIDMÜLLER BCZ 3.81/04/180F</t>
@@ -5024,7 +5024,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5232,7 +5232,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5399,7 +5399,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>223</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>174</v>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>224</v>
@@ -5456,7 +5456,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>223</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>163</v>
@@ -5696,7 +5696,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
100/250RI P7,P8 adjustment; parameter corrections
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="24"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -275,7 +275,7 @@
     <t xml:space="preserve">3 x 10pin MOLEX 5031481090 CLIK-MATE 1.5</t>
   </si>
   <si>
-    <t xml:space="preserve">FE</t>
+    <t xml:space="preserve">FBE</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 12pin MOLEX 5031481290 CLIK-MATE 1.5</t>
@@ -320,7 +320,7 @@
     <t xml:space="preserve">DC BUS (+DC, -DC) –on PCB marked as „VCC, GND“</t>
   </si>
   <si>
-    <t xml:space="preserve">8 x Pressfit M8</t>
+    <t xml:space="preserve">8 x Pressfit M5</t>
   </si>
   <si>
     <t xml:space="preserve">Control, STO</t>
@@ -5231,7 +5231,7 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -7260,7 +7260,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7507,7 +7507,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7758,8 +7758,8 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
TGS/TGZ schematics update, TGZ-D-560-7/15 EN pars. correction
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="317">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -584,6 +584,12 @@
     <t xml:space="preserve">Filter already inside of TGS-560-25/50</t>
   </si>
   <si>
+    <t xml:space="preserve">7,8 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 W</t>
+  </si>
+  <si>
     <t xml:space="preserve">11 kW</t>
   </si>
   <si>
@@ -714,9 +720,6 @@
   </si>
   <si>
     <t xml:space="preserve">Losses at maximum output power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 W</t>
   </si>
   <si>
     <t xml:space="preserve">Recommended circuit breaker</t>
@@ -1258,7 +1261,7 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.92"/>
@@ -1478,7 +1481,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -1714,7 +1717,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -1942,7 +1945,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2178,7 +2181,7 @@
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2403,7 +2406,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2623,7 +2626,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2843,7 +2846,7 @@
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3097,7 +3100,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3351,7 +3354,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3605,7 +3608,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3859,7 +3862,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4087,7 +4090,7 @@
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4328,7 +4331,7 @@
       <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4558,10 +4561,10 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4596,7 +4599,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4604,7 +4607,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4612,7 +4615,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4620,7 +4623,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>171</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4628,7 +4631,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4790,11 +4793,11 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4829,7 +4832,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,7 +4848,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,7 +4856,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,7 +4864,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5030,7 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5044,91 +5047,91 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5143,7 +5146,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -5151,18 +5154,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,12 +5181,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -5191,7 +5194,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>130</v>
@@ -5199,18 +5202,18 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -5235,7 +5238,7 @@
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5252,43 +5255,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -5297,46 +5300,46 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5351,7 +5354,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -5359,18 +5362,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5386,12 +5389,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -5399,7 +5402,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>174</v>
@@ -5407,34 +5410,34 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -5459,7 +5462,7 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5484,16 +5487,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -5502,16 +5505,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -5520,7 +5523,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>56</v>
@@ -5529,7 +5532,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>159</v>
@@ -5538,16 +5541,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -5556,19 +5559,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5583,7 +5586,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5591,18 +5594,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5618,12 +5621,12 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5631,7 +5634,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>163</v>
@@ -5639,15 +5642,15 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>162</v>
@@ -5655,26 +5658,26 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -5699,7 +5702,7 @@
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5716,28 +5719,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5755,19 +5758,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -5782,28 +5785,28 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5821,16 +5824,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -5838,10 +5841,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5849,15 +5852,15 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -5882,7 +5885,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5899,28 +5902,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5965,10 +5968,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -5986,10 +5989,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -5998,7 +6001,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -6007,7 +6010,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
@@ -6018,7 +6021,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6067,7 +6070,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -6084,28 +6087,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -6150,10 +6153,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -6171,10 +6174,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -6183,7 +6186,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -6195,7 +6198,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6228,7 +6231,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -6448,7 +6451,7 @@
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.35"/>
@@ -6463,107 +6466,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6571,16 +6574,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -6606,16 +6609,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -6641,16 +6644,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -6676,16 +6679,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -6711,16 +6714,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -6746,16 +6749,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -6781,16 +6784,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -6816,16 +6819,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -6868,7 +6871,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
@@ -6882,89 +6885,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6984,7 +6987,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -7013,7 +7016,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -7042,7 +7045,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -7071,7 +7074,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -7100,7 +7103,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -7129,7 +7132,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -7163,7 +7166,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
@@ -7173,44 +7176,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7218,7 +7221,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -7232,7 +7235,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>
@@ -7263,7 +7266,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -7510,7 +7513,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.65"/>
@@ -7758,11 +7761,11 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -8014,7 +8017,7 @@
       <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -8242,7 +8245,7 @@
       <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -8478,7 +8481,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>

</xml_diff>

<commit_message>
Added TGZ-S-230-5_15-UNI-RI, other RI corrections and D560-xy FW links
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,25 +21,26 @@
     <sheet name="TGZ-S-48-100_425" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="TGZ-S-48-100_425-O" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="TGZ-S-230-5_15" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="TGZ-D-320-5_10" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="TGZ-D-320-5_15" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="TGZ-S-400-3_9" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="TGZ-S-400-7_15" sheetId="17" state="visible" r:id="rId19"/>
-    <sheet name="TGZ-S-400-10_20" sheetId="18" state="visible" r:id="rId20"/>
-    <sheet name="TGZ-S-400-14_30" sheetId="19" state="visible" r:id="rId21"/>
-    <sheet name="TGZ-D-560-3_9" sheetId="20" state="visible" r:id="rId22"/>
-    <sheet name="TGZ-D-560-7_15" sheetId="21" state="visible" r:id="rId23"/>
-    <sheet name="TGZ-D-560-10_20" sheetId="22" state="visible" r:id="rId24"/>
-    <sheet name="TGZ-D-560-30_50" sheetId="23" state="visible" r:id="rId25"/>
-    <sheet name="TGS-320-10_15" sheetId="24" state="visible" r:id="rId26"/>
-    <sheet name="TGS-560-25_50" sheetId="25" state="visible" r:id="rId27"/>
-    <sheet name="TGS-560-50_100" sheetId="26" state="visible" r:id="rId28"/>
-    <sheet name="TGMmini" sheetId="27" state="visible" r:id="rId29"/>
-    <sheet name="TGMcontroller" sheetId="28" state="visible" r:id="rId30"/>
-    <sheet name="TGZpMotion" sheetId="29" state="visible" r:id="rId31"/>
-    <sheet name="commonHW_DI" sheetId="30" state="visible" r:id="rId32"/>
-    <sheet name="commonHW_DO" sheetId="31" state="visible" r:id="rId33"/>
-    <sheet name="commonHW_AI" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="TGZ-S-230-5_15-UNI-RI" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="TGZ-D-320-5_10" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="TGZ-D-320-5_15" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="TGZ-S-400-3_9" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="TGZ-S-400-7_15" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="TGZ-S-400-10_20" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="TGZ-S-400-14_30" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="TGZ-D-560-3_9" sheetId="21" state="visible" r:id="rId23"/>
+    <sheet name="TGZ-D-560-7_15" sheetId="22" state="visible" r:id="rId24"/>
+    <sheet name="TGZ-D-560-10_20" sheetId="23" state="visible" r:id="rId25"/>
+    <sheet name="TGZ-D-560-30_50" sheetId="24" state="visible" r:id="rId26"/>
+    <sheet name="TGS-320-10_15" sheetId="25" state="visible" r:id="rId27"/>
+    <sheet name="TGS-560-25_50" sheetId="26" state="visible" r:id="rId28"/>
+    <sheet name="TGS-560-50_100" sheetId="27" state="visible" r:id="rId29"/>
+    <sheet name="TGMmini" sheetId="28" state="visible" r:id="rId30"/>
+    <sheet name="TGMcontroller" sheetId="29" state="visible" r:id="rId31"/>
+    <sheet name="TGZpMotion" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="commonHW_DI" sheetId="31" state="visible" r:id="rId33"/>
+    <sheet name="commonHW_DO" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="commonHW_AI" sheetId="33" state="visible" r:id="rId35"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="319">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -419,7 +420,7 @@
     <t xml:space="preserve">1 x 8pin WEIDMÜLLER  B2CF 3.50/08/180</t>
   </si>
   <si>
-    <t xml:space="preserve">EMI FILTR</t>
+    <t xml:space="preserve">EMI FILTER</t>
   </si>
   <si>
     <t xml:space="preserve">Recommended type</t>
@@ -428,6 +429,21 @@
     <t xml:space="preserve">NLMO62P72-04 or NLA062P72-04  </t>
   </si>
   <si>
+    <t xml:space="preserve">-32 ~ +40 °C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 DI, 1 AI, 2 PT1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x green (SERVO OK) 1x red (SERVO ERROR) 1x green (ECAT RUN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 10pin WEIDMÜLLER  BLZP 5.08HC/10/180F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180F  </t>
+  </si>
+  <si>
     <t xml:space="preserve">0-320 VDC (fuse 10 A)</t>
   </si>
   <si>
@@ -471,9 +487,6 @@
   </si>
   <si>
     <t xml:space="preserve">1 x 6pin WEIDMÜLLER  BLF 7.62HP/06/180F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI FILTER</t>
   </si>
   <si>
     <t xml:space="preserve">NCZXX3P49-04</t>
@@ -1105,7 +1118,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1124,6 +1137,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2204,7 +2221,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2430,6 +2447,258 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="68.31"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2467,7 +2736,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2744,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,7 +2760,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2768,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,7 +2861,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>34</v>
@@ -2611,7 +2880,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2896,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,7 +2926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2695,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2703,7 +2972,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,7 +2988,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,7 +3089,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>34</v>
@@ -2839,7 +3108,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +3124,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,7 +3154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2923,7 +3192,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2931,7 +3200,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2939,7 +3208,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,7 +3216,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2960,10 +3229,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,7 +3352,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,7 +3368,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3124,7 +3393,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B31" s="4"/>
     </row>
@@ -3133,269 +3402,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3417,7 +3424,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3439,7 +3446,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3454,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3455,7 +3462,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,7 +3470,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3471,7 +3478,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>150</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,15 +3486,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3607,7 +3614,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3623,7 +3630,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3648,7 +3655,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B31" s="4"/>
     </row>
@@ -3657,7 +3664,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3679,12 +3686,12 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
   </cols>
   <sheetData>
@@ -3701,7 +3708,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,15 +3748,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3869,7 +3876,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3885,7 +3892,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3910,7 +3917,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B31" s="4"/>
     </row>
@@ -3919,7 +3926,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4177,77 +4184,77 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,137 +4273,158 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>163</v>
+      <c r="B25" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>164</v>
+      <c r="B26" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>165</v>
+      <c r="B27" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>166</v>
+      <c r="B28" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="B29" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="A31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>168</v>
+      <c r="B32" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4421,7 +4449,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4440,7 +4468,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4448,7 +4476,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4456,7 +4484,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,7 +4492,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4472,7 +4500,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,7 +4508,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4488,7 +4516,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4592,7 +4620,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4600,7 +4628,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4608,7 +4636,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4616,7 +4644,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4624,12 +4652,12 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4637,7 +4665,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4681,7 +4709,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4689,7 +4717,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,7 +4725,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4705,7 +4733,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4713,7 +4741,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4721,7 +4749,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>173</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,7 +4861,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,7 +4869,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4849,7 +4877,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4857,7 +4885,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4865,12 +4893,12 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4878,7 +4906,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4893,6 +4921,247 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4922,7 +5191,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +5199,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4938,7 +5207,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4946,7 +5215,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,7 +5223,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,7 +5239,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,7 +5343,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5082,7 +5351,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5098,7 +5367,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5106,7 +5375,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5114,12 +5383,12 @@
         <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5396,7 @@
         <v>123</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -5141,7 +5410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5169,46 +5438,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -5217,43 +5486,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -5277,7 +5546,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5285,18 +5554,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5312,12 +5581,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5325,26 +5594,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -5358,7 +5627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5386,43 +5655,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
@@ -5434,43 +5703,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -5494,7 +5763,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5502,18 +5771,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5529,12 +5798,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5542,42 +5811,42 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5591,7 +5860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5622,21 +5891,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>49</v>
@@ -5645,16 +5914,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
@@ -5663,7 +5932,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>59</v>
@@ -5675,22 +5944,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -5699,19 +5968,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C12" s="4"/>
     </row>
@@ -5735,7 +6004,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -5743,18 +6012,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5770,12 +6039,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -5783,242 +6052,50 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -6060,28 +6137,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -6108,19 +6185,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>244</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>245</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>246</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>247</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -6135,84 +6212,82 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>204</v>
+        <v>254</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="C16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>254</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>256</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>105</v>
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>106</v>
+      <c r="A21" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -6231,7 +6306,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
@@ -6254,28 +6329,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -6329,10 +6404,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -6350,10 +6425,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -6362,7 +6437,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -6371,18 +6446,42 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>256</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>254</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -6629,6 +6728,176 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6650,107 +6919,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6758,16 +7027,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -6793,16 +7062,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -6828,16 +7097,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -6863,16 +7132,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -6898,16 +7167,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -6933,16 +7202,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -6968,16 +7237,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -7003,16 +7272,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -7044,7 +7313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7069,89 +7338,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7171,7 +7440,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -7200,7 +7469,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -7229,7 +7498,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -7258,7 +7527,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -7287,7 +7556,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -7316,7 +7585,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -7339,7 +7608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7360,44 +7629,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7405,7 +7674,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -7419,7 +7688,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>
@@ -7702,7 +7971,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7962,7 +8231,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
TGmonitor added. Some chapters missing temporarily (dim, mount...)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,6 +45,7 @@
     <sheet name="commonHW_DI" sheetId="35" state="visible" r:id="rId37"/>
     <sheet name="commonHW_DO" sheetId="36" state="visible" r:id="rId38"/>
     <sheet name="commonHW_AI" sheetId="37" state="visible" r:id="rId39"/>
+    <sheet name="TGmonitor7" sheetId="38" state="visible" r:id="rId40"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="340">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -1040,13 +1041,78 @@
   <si>
     <t xml:space="preserve">us</t>
   </si>
+  <si>
+    <t xml:space="preserve">Supply voltage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommended PSU current </t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. 300 mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPLAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 inches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viewing Angles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1024 x 600 pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Area Dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">154.21 x 85.92 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pixel Pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150.6 µm (H) x 143.2 µm (V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color Gamut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45% NTSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Brightness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 cd/m²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrast Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800:1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00\ %"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1122,7 +1188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1141,6 +1207,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5159,8 +5237,8 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7321,7 +7399,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8684,6 +8762,168 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
renamed xyzRI by xyz-RI
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -11,11 +11,11 @@
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="TGZ-D-48-50_100" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="TGZ-S-48-50_100" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="TGZ-S-48-50_100RI" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="TGZ-S-48-50_100-RI" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="TGZ-S-48-50_100-UNI-RI" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="TGZ-S-48-100_250RI" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="TGZ-S-48-100_250-RI" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="TGZ-S-48-100_250-UNI-RI" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="TGZ-S-48-100_300RI" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="TGZ-S-48-100_300-RI" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="TGZ-S-48-100_300-UNI-RI" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="TGZ-S-48-100_250" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="TGZ-S-48-100_250-O" sheetId="11" state="visible" r:id="rId13"/>
@@ -9248,7 +9248,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10405,7 +10405,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
upravy CommonHW, preklady, pridany linky do sekce z RI serv
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="39"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="38"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="339">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -987,9 +987,6 @@
   </si>
   <si>
     <t xml:space="preserve"> I&lt;sub&gt;O,max&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Osa č. </t>
   </si>
   <si>
     <t xml:space="preserve"> f&lt;sub&gt;maxSq&lt;/sub&gt;</t>
@@ -9239,8 +9236,8 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9307,10 +9304,10 @@
         <v>308</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9359,7 +9356,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -9388,7 +9385,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -9417,7 +9414,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -9446,7 +9443,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -9475,7 +9472,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -9504,7 +9501,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -9773,7 +9770,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -9790,13 +9787,13 @@
         <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9804,13 +9801,13 @@
         <v>273</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9824,7 +9821,7 @@
         <v>288</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9894,7 +9891,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>240</v>
@@ -9902,10 +9899,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9935,7 +9932,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>257</v>
@@ -9944,7 +9941,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -9952,66 +9949,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
S-48-100/300 peak current set to 350A in all versions
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="38"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -15,12 +15,12 @@
     <sheet name="TGZ-S-48-50_100-UNI-RI" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="TGZ-S-48-100_250-RI" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="TGZ-S-48-100_250-UNI-RI" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="TGZ-S-48-100_300-RI" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="TGZ-S-48-100_300-UNI-RI" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="TGZ-S-48-100_250" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="TGZ-S-48-100_250-O" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="TGZ-S-48-100_300" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="TGZ-S-48-100_300-O" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="TGZ-S-48-100_300" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="TGZ-S-48-100_300-RI" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="TGZ-S-48-100_300-UNI-RI" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="TGZ-S-48-100_300-O" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="TGZ-S-48-100_250" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="TGZ-S-48-100_250-O" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="TGZ-S-48-100_425" sheetId="14" state="visible" r:id="rId16"/>
     <sheet name="TGZ-S-48-100_425-O" sheetId="15" state="visible" r:id="rId17"/>
     <sheet name="TGZ-S-230-5_15" sheetId="16" state="visible" r:id="rId18"/>
@@ -359,7 +359,13 @@
     <t xml:space="preserve">1 x 4pin MOLEX Micro-Fit 3.0, 430250400</t>
   </si>
   <si>
-    <t xml:space="preserve">300 A</t>
+    <t xml:space="preserve">350 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 x Pressfit M5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin MOLEX Micro-Fit 3.0, 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">External thermistor</t>
@@ -371,28 +377,22 @@
     <t xml:space="preserve">1x green (SERVO OK) 1x red (SERVO ERROR)</t>
   </si>
   <si>
-    <t xml:space="preserve">8 x Pressfit M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 5pin MOLEX Micro-Fit 3.0, 436450500</t>
+    <t xml:space="preserve">2x terminal DIN Molex 201606-0610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x terminal DIN WEIDMÜLLER WDU 1.5/R3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3x terminal DIN Molex 201606-6163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4x terminal DIN WEIDMÜLLER WDU 1.5/R3.5</t>
   </si>
   <si>
     <t xml:space="preserve">2 x 8pin WEIDMÜLLER  B2CF 3.50/08/180</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 12pin WEIDMÜLLER  B2CF 3.50/12/180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2x terminal DIN Molex 201606-0610</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2x terminal DIN WEIDMÜLLER WDU 1.5/R3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3x terminal DIN Molex 201606-6163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4x terminal DIN WEIDMÜLLER WDU 1.5/R3.5</t>
   </si>
   <si>
     <t xml:space="preserve">STO A, B</t>
@@ -1568,15 +1568,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
@@ -1625,7 +1625,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,7 +1649,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,7 +1665,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1673,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,12 +1681,12 @@
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -1694,98 +1694,122 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1806,8 +1830,8 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1861,7 +1885,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,7 +1957,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,7 +1981,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,7 +1997,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,7 +2005,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +2013,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,7 +2021,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,7 +2029,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,15 +2037,15 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,7 +2053,7 @@
         <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2056,7 +2080,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
@@ -2105,7 +2129,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,7 +2201,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,8 +2224,8 @@
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>34</v>
+      <c r="B21" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,7 +2241,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2249,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,7 +2273,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,12 +2281,12 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>97</v>
@@ -2341,7 +2365,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,7 +2437,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,7 +2461,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2453,7 +2477,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,7 +2485,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,7 +2493,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,7 +2501,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,7 +2509,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,15 +2517,15 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2533,7 @@
         <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2697,7 +2721,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +2729,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2766,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>97</v>
@@ -2893,7 +2917,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,7 +2941,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2933,7 +2957,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,7 +2965,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,7 +2973,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2957,7 +2981,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +2989,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,15 +2997,15 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,7 +3013,7 @@
         <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3209,7 +3233,7 @@
         <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4670,7 +4694,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4678,7 +4702,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4898,7 +4922,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +4930,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -5150,7 +5174,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5412,7 +5436,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,7 +5698,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5936,7 +5960,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8223,7 +8247,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8231,7 +8255,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8239,7 +8263,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -8409,7 +8433,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -9236,7 +9260,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -10786,15 +10810,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
@@ -10835,7 +10859,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10867,7 +10891,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10880,138 +10904,130 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="1" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -11030,10 +11046,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11079,7 +11095,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11124,153 +11140,137 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="1" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TGZ-S-48-100/xyz log pwr connector error cleared microfit instead of microlock
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="341">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -346,7 +346,7 @@
     <t xml:space="preserve">Control, STO</t>
   </si>
   <si>
-    <t xml:space="preserve">1 x 5pin MOLEX Micro-Lock, 5055700501</t>
+    <t xml:space="preserve">1 x 5pin Molex Micro-Fit 3.0 - 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">3 x Pressfit M8</t>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t xml:space="preserve">8 x Pressfit M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 5pin MOLEX Micro-Fit 3.0, 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">External thermistor</t>
@@ -1582,7 +1579,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1793,7 +1790,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>97</v>
@@ -1826,7 +1823,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2053,7 +2050,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>97</v>
@@ -2086,7 +2083,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2212,7 +2209,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,7 +2233,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,7 +2249,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2260,7 +2257,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2265,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,7 +2273,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2281,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,23 +2289,23 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2330,7 +2327,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2456,7 +2453,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +2477,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,7 +2501,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2525,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2536,12 +2533,12 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>97</v>
@@ -2692,7 +2689,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2716,7 +2713,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2732,7 +2729,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,7 +2737,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,7 +2745,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,7 +2753,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,7 +2761,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,23 +2769,23 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2809,8 +2806,8 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2864,7 +2861,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +2981,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3021,7 +3018,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>97</v>
@@ -3100,7 +3097,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3172,7 +3169,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,7 +3193,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3212,7 +3209,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3220,7 +3217,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,7 +3225,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3236,7 +3233,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,7 +3241,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,23 +3249,23 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3312,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,7 +3317,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3328,7 +3325,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3336,7 +3333,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3352,7 +3349,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,7 +3453,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3464,7 +3461,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3469,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3480,7 +3477,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,20 +3485,20 @@
         <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3545,7 +3542,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3553,7 +3550,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3561,7 +3558,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,7 +3566,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,7 +3582,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3689,7 +3686,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3697,7 +3694,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,7 +3702,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3713,7 +3710,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3721,20 +3718,20 @@
         <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3778,7 +3775,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,7 +3783,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3794,7 +3791,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,7 +3799,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,7 +3815,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,7 +3831,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3887,7 +3884,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>72</v>
@@ -3940,7 +3937,7 @@
         <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3957,7 +3954,7 @@
         <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,7 +3962,7 @@
         <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3973,20 +3970,20 @@
         <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4266,7 +4263,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,7 +4271,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,7 +4279,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4290,7 +4287,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,7 +4303,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,7 +4319,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4359,7 +4356,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>72</v>
@@ -4412,7 +4409,7 @@
         <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4429,7 +4426,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4437,7 +4434,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4445,20 +4442,20 @@
         <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4510,7 +4507,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4515,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,7 +4523,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,7 +4531,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4542,15 +4539,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4566,7 +4563,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4616,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>72</v>
@@ -4672,7 +4669,7 @@
         <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4689,7 +4686,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,7 +4694,7 @@
         <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4705,20 +4702,20 @@
         <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4770,7 +4767,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4778,7 +4775,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +4783,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4794,7 +4791,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4802,15 +4799,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,7 +4823,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4863,7 +4860,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>72</v>
@@ -4916,7 +4913,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4933,7 +4930,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,7 +4938,7 @@
         <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4949,20 +4946,20 @@
         <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5014,7 +5011,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5022,7 +5019,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5030,7 +5027,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5038,7 +5035,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5046,7 +5043,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5139,7 +5136,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>34</v>
@@ -5158,7 +5155,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5166,7 +5163,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,7 +5171,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5182,7 +5179,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5190,7 +5187,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -5242,7 +5239,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5250,7 +5247,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5258,7 +5255,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5266,7 +5263,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5367,7 +5364,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>34</v>
@@ -5386,7 +5383,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5394,7 +5391,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5402,7 +5399,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5410,7 +5407,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5418,7 +5415,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -5470,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5478,7 +5475,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5486,7 +5483,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5494,7 +5491,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5507,10 +5504,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5618,7 +5615,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5626,7 +5623,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5634,7 +5631,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,7 +5639,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5650,21 +5647,21 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5716,7 +5713,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5724,7 +5721,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5732,7 +5729,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5753,10 +5750,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5864,7 +5861,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5872,7 +5869,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5880,7 +5877,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5888,7 +5885,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5896,21 +5893,21 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5954,7 +5951,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5962,7 +5959,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5970,7 +5967,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5978,7 +5975,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5986,7 +5983,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5999,10 +5996,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6110,7 +6107,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6118,7 +6115,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6126,7 +6123,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6134,7 +6131,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6142,21 +6139,21 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -6208,7 +6205,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6216,7 +6213,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6224,7 +6221,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6232,7 +6229,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6240,15 +6237,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6356,7 +6353,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6364,7 +6361,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6372,7 +6369,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6380,7 +6377,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6388,21 +6385,21 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -6446,7 +6443,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6454,7 +6451,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6462,7 +6459,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6470,7 +6467,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6478,7 +6475,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6486,7 +6483,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6494,7 +6491,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6598,7 +6595,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6606,7 +6603,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,7 +6611,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6622,7 +6619,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6630,20 +6627,20 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -6915,7 +6912,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6923,7 +6920,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6931,7 +6928,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6939,7 +6936,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6947,7 +6944,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6963,7 +6960,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7067,7 +7064,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7075,7 +7072,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7083,7 +7080,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7091,7 +7088,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7099,20 +7096,20 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -7156,7 +7153,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7164,7 +7161,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7172,7 +7169,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7180,7 +7177,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7188,7 +7185,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7196,7 +7193,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7204,7 +7201,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7308,7 +7305,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7316,7 +7313,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7324,7 +7321,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7332,7 +7329,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7340,20 +7337,20 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -7397,7 +7394,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7405,7 +7402,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7413,7 +7410,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7421,7 +7418,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7429,7 +7426,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7445,7 +7442,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7549,7 +7546,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7557,7 +7554,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7573,7 +7570,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7581,7 +7578,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7589,20 +7586,20 @@
         <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -7644,46 +7641,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -7692,43 +7689,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -7752,7 +7749,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -7760,18 +7757,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7787,12 +7784,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -7800,26 +7797,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -7861,43 +7858,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -7909,43 +7906,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -7969,7 +7966,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -7977,18 +7974,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8004,12 +8001,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -8017,42 +8014,42 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -8097,21 +8094,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
@@ -8120,16 +8117,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -8138,7 +8135,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>59</v>
@@ -8150,22 +8147,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -8174,19 +8171,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -8210,7 +8207,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -8218,18 +8215,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8245,12 +8242,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -8258,50 +8255,50 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -8343,28 +8340,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -8391,19 +8388,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -8418,28 +8415,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -8457,16 +8454,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -8474,10 +8471,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8485,15 +8482,15 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -8535,28 +8532,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -8610,10 +8607,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -8631,10 +8628,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -8643,7 +8640,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -8652,7 +8649,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>39</v>
@@ -8663,7 +8660,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8671,7 +8668,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8679,7 +8676,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8687,7 +8684,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -8729,28 +8726,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -8804,10 +8801,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -8825,10 +8822,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -8837,7 +8834,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -8849,7 +8846,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8857,7 +8854,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -8897,107 +8894,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9005,16 +9002,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.05</v>
@@ -9040,16 +9037,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.05</v>
@@ -9075,16 +9072,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2.05</v>
@@ -9110,16 +9107,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2.05</v>
@@ -9145,16 +9142,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2.05</v>
@@ -9180,16 +9177,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.05</v>
@@ -9215,16 +9212,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1.25</v>
@@ -9250,16 +9247,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>1.25</v>
@@ -9555,98 +9552,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9654,10 +9651,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
@@ -9686,10 +9683,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
@@ -9718,10 +9715,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
@@ -9750,10 +9747,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
@@ -9782,10 +9779,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
@@ -9814,10 +9811,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
@@ -9846,10 +9843,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
@@ -9878,10 +9875,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
@@ -9941,89 +9938,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>290</v>
-      </c>
       <c r="H3" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10043,7 +10040,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>300</v>
@@ -10072,7 +10069,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>300</v>
@@ -10101,7 +10098,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>300</v>
@@ -10130,7 +10127,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>300</v>
@@ -10159,7 +10156,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>300</v>
@@ -10188,7 +10185,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>300</v>
@@ -10232,44 +10229,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10277,7 +10274,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>11</v>
@@ -10291,7 +10288,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>11</v>
@@ -10339,24 +10336,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -10364,32 +10361,32 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -10397,66 +10394,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>336</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -10733,7 +10730,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10977,7 +10974,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11236,8 +11233,8 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11505,7 +11502,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11679,7 +11676,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11716,7 +11713,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
smartBrake matplotlib python test (plot folder in source)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.en.xlsx
+++ b/docs/Manual/source/tab/parameters.en.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="345">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t xml:space="preserve">4 x 10pin MOLEX 5031481090 CLIK-MATE 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC16XXX</t>
   </si>
   <si>
     <t xml:space="preserve">0-320 VDC (fuse 10 A)</t>
@@ -4747,7 +4750,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4985,7 +4988,7 @@
         <v>124</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -5281,7 +5284,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,7 +5292,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5305,7 +5308,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5313,7 +5316,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5406,7 +5409,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>34</v>
@@ -5425,7 +5428,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5441,7 +5444,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5509,7 +5512,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5517,7 +5520,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5533,7 +5536,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5634,7 +5637,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>34</v>
@@ -5653,7 +5656,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5669,7 +5672,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,7 +5740,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5745,7 +5748,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5753,7 +5756,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5761,7 +5764,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5774,10 +5777,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5983,7 +5986,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5991,7 +5994,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6023,7 +6026,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6221,7 +6224,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6229,7 +6232,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,7 +6240,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6245,7 +6248,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6253,7 +6256,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6269,7 +6272,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6941,7 +6944,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6957,7 +6960,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6965,7 +6968,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6973,7 +6976,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6981,7 +6984,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6989,7 +6992,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7093,7 +7096,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7101,7 +7104,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7109,7 +7112,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7117,7 +7120,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7125,7 +7128,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7138,7 +7141,7 @@
         <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -7182,7 +7185,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7198,7 +7201,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7230,7 +7233,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7334,7 +7337,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7342,7 +7345,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7350,7 +7353,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7358,7 +7361,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7366,7 +7369,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,7 +7382,7 @@
         <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -7423,7 +7426,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7439,7 +7442,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7447,7 +7450,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7455,7 +7458,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7463,7 +7466,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7471,7 +7474,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7575,7 +7578,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7583,7 +7586,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7591,7 +7594,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7599,7 +7602,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7607,7 +7610,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7620,7 +7623,7 @@
         <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -7664,7 +7667,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7680,7 +7683,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7696,7 +7699,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7712,7 +7715,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7816,7 +7819,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7824,7 +7827,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7840,7 +7843,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7848,7 +7851,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7856,7 +7859,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7869,7 +7872,7 @@
         <v>124</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -7911,46 +7914,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -7959,43 +7962,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -8019,7 +8022,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -8027,18 +8030,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8054,12 +8057,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -8067,26 +8070,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -8128,43 +8131,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -8176,43 +8179,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -8236,7 +8239,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -8244,18 +8247,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8271,12 +8274,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -8284,42 +8287,42 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -8364,21 +8367,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
@@ -8387,16 +8390,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -8405,7 +8408,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>59</v>
@@ -8417,22 +8420,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -8441,19 +8444,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -8477,7 +8480,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -8485,18 +8488,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8512,12 +8515,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -8525,50 +8528,50 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -8610,28 +8613,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -8658,19 +8661,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -8685,28 +8688,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -8724,16 +8727,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -8741,10 +8744,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8752,15 +8755,15 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -8802,28 +8805,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -8877,10 +8880,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -8898,10 +8901,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -8910,7 +8913,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -8919,7 +8922,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>39</v>
@@ -8930,7 +8933,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8996,28 +8999,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -9071,10 +9074,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -9092,10 +9095,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -9104,7 +9107,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -9116,7 +9119,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9403,107 +9406,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9511,16 +9514,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.05</v>
@@ -9546,16 +9549,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.05</v>
@@ -9581,16 +9584,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2.05</v>
@@ -9616,16 +9619,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2.05</v>
@@ -9651,16 +9654,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2.05</v>
@@ -9686,16 +9689,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.05</v>
@@ -9721,16 +9724,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1.25</v>
@@ -9756,16 +9759,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>1.25</v>
@@ -9822,98 +9825,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9921,10 +9924,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
@@ -9953,10 +9956,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
@@ -9985,10 +9988,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
@@ -10017,10 +10020,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
@@ -10049,10 +10052,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
@@ -10081,10 +10084,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
@@ -10113,10 +10116,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
@@ -10145,10 +10148,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
@@ -10208,89 +10211,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10310,7 +10313,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>300</v>
@@ -10339,7 +10342,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>300</v>
@@ -10368,7 +10371,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>300</v>
@@ -10397,7 +10400,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>300</v>
@@ -10426,7 +10429,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>300</v>
@@ -10455,7 +10458,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>300</v>
@@ -10499,44 +10502,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10544,7 +10547,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>11</v>
@@ -10558,7 +10561,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>11</v>
@@ -10606,24 +10609,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -10631,32 +10634,32 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -10664,66 +10667,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>